<commit_message>
Tested Player and Card classes
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Bug</t>
   </si>
@@ -20,22 +22,79 @@
   </si>
   <si>
     <t>Fix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">takeDamage() method assigns taken damage as new hp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When user takes damage his new HP gets the value of taken damage instead of HP=HP-takenDamage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add health-=amountOfDamage to takeDamage() method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BoostAttackCard method getBoost() returns 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instead of returning 3, getBoost return 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">replace return number with return boost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">damage does not reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When resetDamage is called, player's damage is not reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">replace damage = damage with damage = 0 in resetDamage() method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shufle doesn't do anything</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemented shuffle algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">findNumberInHand returns wrong value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instead of returnig true when card is found it return false and vice versa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switch return statment places</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cardToPlay is not null checked </t>
+  </si>
+  <si>
+    <t xml:space="preserve">application crashes because null is passed to cardToPlay.effect()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check if null and notifiy user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player health drops below zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is no limit to how low Player HP can drop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
+      <sz val="10.000000"/>
+      <color indexed="64"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <color rgb="FFFFFFFF"/>
+      <color indexed="65"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -44,7 +103,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -54,35 +113,321 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+  <cellXfs count="2">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -139,7 +484,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -165,7 +510,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -217,16 +562,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -242,7 +599,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -272,39 +629,115 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr applyStyles="0" summaryBelow="0" summaryRight="0" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.630000000000001" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="36.25"/>
-    <col customWidth="1" min="2" max="2" width="36.13"/>
-    <col customWidth="1" min="3" max="3" width="41.63"/>
+    <col customWidth="1" min="1" max="1" width="59.00390625"/>
+    <col customWidth="1" min="2" max="2" width="78.140625"/>
+    <col customWidth="1" min="3" max="3" width="70.8515625"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished testing Game class
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Bug</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t xml:space="preserve">There is no limit to how low Player HP can drop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP is set to zero if incoming damage is greater than HP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Game does not end if a player's HP reached 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player is asked for turn input before HP check is done to end the game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moved HP check code to execute before player turn starts</t>
   </si>
 </sst>
 </file>
@@ -88,7 +100,7 @@
   <fonts count="2">
     <font>
       <sz val="10.000000"/>
-      <color indexed="64"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -647,8 +659,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.630000000000001" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="59.00390625"/>
-    <col customWidth="1" min="2" max="2" width="78.140625"/>
+    <col customWidth="1" min="1" max="1" width="77.421875"/>
+    <col customWidth="1" min="2" max="2" width="100.421875"/>
     <col customWidth="1" min="3" max="3" width="70.8515625"/>
   </cols>
   <sheetData>
@@ -733,7 +745,22 @@
       <c r="B8" t="s">
         <v>21</v>
       </c>
-    </row>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>